<commit_message>
Resolved some early issues, added some feature requests
</commit_message>
<xml_diff>
--- a/Tests/Bug Database.xlsx
+++ b/Tests/Bug Database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47350DC7-7141-4B01-92D4-A4697885EFCB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3F0BFF-EA54-48CC-B068-7B52B38BA623}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Complete Steps to Reproduce</t>
   </si>
@@ -80,13 +80,43 @@
   </si>
   <si>
     <t>No unit tests currently in the Tests/Unit folder</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>Resolution Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I've renamed and cleaned up the search log function.  The way it operates is more consistent, predictable, and clean. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">search_log() has been updated and it no longer allows you to choose the log database.  It uses the same database each time, which is the desired functionality. </t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One unit test has been added, more are needed. </t>
+  </si>
+  <si>
+    <t>FR: Allow switch between horizontal and vertical seperatation in GUI</t>
+  </si>
+  <si>
+    <t>Allow the user to choose whether to have a horizontal or vertical split in the gui</t>
+  </si>
+  <si>
+    <t>FR: Highlight problem messages with pretty colors</t>
+  </si>
+  <si>
+    <t>FR: Clicking a problem message in the scanned log side should scroll the other side to the problem message</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,13 +132,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -120,10 +162,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -131,8 +174,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -411,20 +463,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="28.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="28.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -443,48 +495,57 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
+      <c r="F2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:7" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
+      <c r="F3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -501,6 +562,69 @@
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>